<commit_message>
fuel boiler efficiency set in the excel input table
</commit_message>
<xml_diff>
--- a/tests/operation/input/OperationScenario_Component_Boiler.xlsx
+++ b/tests/operation/input/OperationScenario_Component_Boiler.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/FLEX/tests/operation/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7447C9C-17B9-4D40-908D-6F06D0BA6D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C35CB-8DD6-FE45-95E6-7921B421F316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="3700" windowWidth="23480" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-460" yWindow="-21860" windowWidth="32080" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Boi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>ID_Boiler</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>liquids</t>
+  </si>
+  <si>
+    <t>fuel_boiler_efficiency</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="258" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -907,7 +910,7 @@
     <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -923,8 +926,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -940,8 +946,11 @@
       <c r="E2">
         <v>0.35</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -957,8 +966,11 @@
       <c r="E3">
         <v>0.35</v>
       </c>
+      <c r="F3">
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -974,8 +986,11 @@
       <c r="E4">
         <v>0.35</v>
       </c>
+      <c r="F4">
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -991,8 +1006,11 @@
       <c r="E5">
         <v>0.35</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1007,6 +1025,9 @@
       </c>
       <c r="E6">
         <v>0.35</v>
+      </c>
+      <c r="F6">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>